<commit_message>
heroes typo 'The Hero'
</commit_message>
<xml_diff>
--- a/tvTropesSSheet.xlsx
+++ b/tvTropesSSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="363">
   <si>
     <t>Identifier</t>
   </si>
@@ -1121,6 +1121,9 @@
   </si>
   <si>
     <t>Freud Was Right</t>
+  </si>
+  <si>
+    <t>The Hero</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2209,7 @@
         <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>362</v>
       </c>
       <c r="C53" t="s">
         <v>60</v>

</xml_diff>